<commit_message>
Update and reorganize excel spreadsheets
</commit_message>
<xml_diff>
--- a/CurrentData/Raw Edgelists_Excel/SLR_raw_barriers.xlsx
+++ b/CurrentData/Raw Edgelists_Excel/SLR_raw_barriers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyras\OneDrive\Desktop\SLRSurvey\SLRSurvey\CurrentData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyras\OneDrive\Desktop\SLRSurvey\SLRSurvey\CurrentData\Raw Edgelists_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="28">
   <si>
     <t>Barrier1</t>
   </si>
@@ -79,6 +79,36 @@
   <si>
     <t>Sci Info</t>
   </si>
+  <si>
+    <t>Openness</t>
+  </si>
+  <si>
+    <t>Urgency/Priority</t>
+  </si>
+  <si>
+    <t>Existing Policies</t>
+  </si>
+  <si>
+    <t>Info Share/Use</t>
+  </si>
+  <si>
+    <t>Reg Leader</t>
+  </si>
+  <si>
+    <t>Competition</t>
+  </si>
+  <si>
+    <t>Stakeholder Engage/Influence</t>
+  </si>
+  <si>
+    <t>Outside Scope</t>
+  </si>
+  <si>
+    <t>Narrow Grey Focus</t>
+  </si>
+  <si>
+    <t>Partner Capacity</t>
+  </si>
 </sst>
 </file>
 
@@ -113,8 +143,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,7 +429,7 @@
   <dimension ref="A1:C869"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,12 +472,12 @@
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -484,7 +515,7 @@
         <v>7</v>
       </c>
       <c r="C89" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -518,9 +549,6 @@
       <c r="B124" t="s">
         <v>13</v>
       </c>
-      <c r="C124" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
@@ -557,7 +585,7 @@
         <v>7</v>
       </c>
       <c r="C128" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -644,7 +672,7 @@
         <v>6</v>
       </c>
       <c r="C138" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -703,7 +731,7 @@
         <v>6</v>
       </c>
       <c r="B145" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -745,9 +773,6 @@
       <c r="B151" t="s">
         <v>3</v>
       </c>
-      <c r="C151" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
@@ -848,7 +873,7 @@
         <v>7</v>
       </c>
       <c r="C164" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -894,7 +919,7 @@
         <v>16</v>
       </c>
       <c r="B169" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -924,7 +949,7 @@
         <v>6</v>
       </c>
       <c r="B173" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -946,7 +971,7 @@
         <v>6</v>
       </c>
       <c r="C175" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -1009,7 +1034,7 @@
         <v>6</v>
       </c>
       <c r="C181" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -1120,7 +1145,7 @@
         <v>6</v>
       </c>
       <c r="C194" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -1136,7 +1161,7 @@
         <v>16</v>
       </c>
       <c r="B196" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -1247,7 +1272,7 @@
         <v>11</v>
       </c>
       <c r="B209" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -1258,7 +1283,7 @@
         <v>3</v>
       </c>
       <c r="C210" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -1285,7 +1310,7 @@
         <v>6</v>
       </c>
       <c r="C213" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -1382,7 +1407,7 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -1444,7 +1469,7 @@
         <v>7</v>
       </c>
       <c r="B233" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -1495,7 +1520,7 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -1612,11 +1637,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A259" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>5</v>
@@ -1647,7 +1667,7 @@
         <v>6</v>
       </c>
       <c r="C262" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -1695,7 +1715,7 @@
         <v>16</v>
       </c>
       <c r="B268" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -1797,7 +1817,7 @@
         <v>3</v>
       </c>
       <c r="B280" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -1892,16 +1912,13 @@
         <v>3</v>
       </c>
       <c r="B290" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>3</v>
       </c>
-      <c r="B292" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
@@ -1919,7 +1936,7 @@
         <v>5</v>
       </c>
       <c r="C294" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
@@ -1951,7 +1968,7 @@
         <v>13</v>
       </c>
       <c r="C298" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
@@ -1973,7 +1990,7 @@
         <v>16</v>
       </c>
       <c r="C300" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
@@ -1983,6 +2000,9 @@
       <c r="B301" t="s">
         <v>10</v>
       </c>
+      <c r="C301" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
@@ -1997,7 +2017,7 @@
         <v>3</v>
       </c>
       <c r="B303" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
@@ -2182,7 +2202,7 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
@@ -2250,7 +2270,7 @@
         <v>13</v>
       </c>
       <c r="C331" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
@@ -2274,7 +2294,7 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
@@ -2325,7 +2345,7 @@
         <v>6</v>
       </c>
       <c r="B340" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
@@ -2446,7 +2466,7 @@
         <v>9</v>
       </c>
       <c r="C354" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
@@ -2466,9 +2486,6 @@
       </c>
       <c r="B356" t="s">
         <v>7</v>
-      </c>
-      <c r="C356" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
@@ -2516,9 +2533,6 @@
       <c r="A361" t="s">
         <v>3</v>
       </c>
-      <c r="B361" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
@@ -2694,7 +2708,7 @@
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
@@ -2740,12 +2754,12 @@
         <v>7</v>
       </c>
       <c r="C387" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
@@ -2826,9 +2840,6 @@
       <c r="B396" t="s">
         <v>13</v>
       </c>
-      <c r="C396" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
@@ -2854,7 +2865,7 @@
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
@@ -2870,7 +2881,7 @@
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.25">
@@ -3015,7 +3026,7 @@
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.25">
@@ -3068,9 +3079,6 @@
       <c r="B427" t="s">
         <v>3</v>
       </c>
-      <c r="C427" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
@@ -3091,7 +3099,7 @@
         <v>17</v>
       </c>
       <c r="C429" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.25">
@@ -3142,7 +3150,7 @@
         <v>3</v>
       </c>
       <c r="B436" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.25">
@@ -3221,7 +3229,7 @@
         <v>6</v>
       </c>
       <c r="C444" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.25">
@@ -3253,7 +3261,7 @@
         <v>5</v>
       </c>
       <c r="C448" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.25">
@@ -3365,7 +3373,7 @@
         <v>5</v>
       </c>
       <c r="C460" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.25">
@@ -3422,7 +3430,7 @@
         <v>6</v>
       </c>
       <c r="C466" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="467" spans="1:3" x14ac:dyDescent="0.25">
@@ -3433,7 +3441,7 @@
         <v>6</v>
       </c>
       <c r="C467" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="468" spans="1:3" x14ac:dyDescent="0.25">
@@ -3444,7 +3452,7 @@
         <v>6</v>
       </c>
       <c r="C468" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.25">
@@ -3476,7 +3484,7 @@
     </row>
     <row r="472" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="473" spans="1:3" x14ac:dyDescent="0.25">
@@ -3515,9 +3523,6 @@
       <c r="A477" t="s">
         <v>6</v>
       </c>
-      <c r="B477" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="478" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
@@ -3578,11 +3583,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="485" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A485" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>11</v>
@@ -3678,7 +3678,7 @@
         <v>6</v>
       </c>
       <c r="C499" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="500" spans="1:3" x14ac:dyDescent="0.25">
@@ -3739,7 +3739,7 @@
         <v>3</v>
       </c>
       <c r="B507" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="508" spans="1:3" x14ac:dyDescent="0.25">
@@ -3859,7 +3859,13 @@
     </row>
     <row r="523" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="B523" t="s">
+        <v>3</v>
+      </c>
+      <c r="C523" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="524" spans="1:3" x14ac:dyDescent="0.25">
@@ -4076,7 +4082,7 @@
         <v>3</v>
       </c>
       <c r="C547" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="548" spans="1:3" x14ac:dyDescent="0.25">
@@ -4116,7 +4122,7 @@
     </row>
     <row r="552" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="553" spans="1:3" x14ac:dyDescent="0.25">
@@ -4188,7 +4194,7 @@
         <v>16</v>
       </c>
       <c r="C561" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="562" spans="1:3" x14ac:dyDescent="0.25">
@@ -4204,7 +4210,7 @@
         <v>3</v>
       </c>
       <c r="B564" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="565" spans="1:3" x14ac:dyDescent="0.25">
@@ -4227,7 +4233,7 @@
     </row>
     <row r="568" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="569" spans="1:3" x14ac:dyDescent="0.25">
@@ -4238,7 +4244,7 @@
         <v>16</v>
       </c>
       <c r="C569" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="570" spans="1:3" x14ac:dyDescent="0.25">
@@ -4330,7 +4336,7 @@
         <v>9</v>
       </c>
       <c r="C579" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="580" spans="1:3" x14ac:dyDescent="0.25">
@@ -4367,7 +4373,7 @@
         <v>16</v>
       </c>
       <c r="C584" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="585" spans="1:3" x14ac:dyDescent="0.25">
@@ -4388,7 +4394,7 @@
     </row>
     <row r="587" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="588" spans="1:3" x14ac:dyDescent="0.25">
@@ -4406,7 +4412,10 @@
     </row>
     <row r="590" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
-        <v>10</v>
+        <v>25</v>
+      </c>
+      <c r="B590" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="591" spans="1:3" x14ac:dyDescent="0.25">
@@ -4441,12 +4450,12 @@
         <v>6</v>
       </c>
       <c r="C594" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="595" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="596" spans="1:3" x14ac:dyDescent="0.25">
@@ -4628,7 +4637,7 @@
         <v>16</v>
       </c>
       <c r="C615" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="616" spans="1:3" x14ac:dyDescent="0.25">
@@ -4639,7 +4648,7 @@
         <v>6</v>
       </c>
       <c r="C616" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="617" spans="1:3" x14ac:dyDescent="0.25">
@@ -4687,7 +4696,7 @@
         <v>3</v>
       </c>
       <c r="B622" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="623" spans="1:3" x14ac:dyDescent="0.25">
@@ -4695,7 +4704,7 @@
         <v>11</v>
       </c>
       <c r="B623" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="624" spans="1:3" x14ac:dyDescent="0.25">
@@ -4725,7 +4734,7 @@
         <v>6</v>
       </c>
       <c r="B626" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="627" spans="1:3" x14ac:dyDescent="0.25">
@@ -4741,7 +4750,7 @@
     </row>
     <row r="628" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="630" spans="1:3" x14ac:dyDescent="0.25">
@@ -4756,7 +4765,7 @@
     </row>
     <row r="632" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A632" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="634" spans="1:3" x14ac:dyDescent="0.25">
@@ -4775,7 +4784,7 @@
         <v>5</v>
       </c>
       <c r="B635" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="636" spans="1:3" x14ac:dyDescent="0.25">
@@ -4832,7 +4841,7 @@
         <v>16</v>
       </c>
       <c r="C641" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="642" spans="1:3" x14ac:dyDescent="0.25">
@@ -4913,7 +4922,7 @@
         <v>14</v>
       </c>
       <c r="B651" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="652" spans="1:3" x14ac:dyDescent="0.25">
@@ -4974,7 +4983,7 @@
         <v>3</v>
       </c>
       <c r="B659" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="660" spans="1:3" x14ac:dyDescent="0.25">
@@ -5022,7 +5031,7 @@
         <v>6</v>
       </c>
       <c r="C666" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="667" spans="1:3" x14ac:dyDescent="0.25">
@@ -5119,7 +5128,7 @@
         <v>3</v>
       </c>
       <c r="C677" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="678" spans="1:3" x14ac:dyDescent="0.25">
@@ -5219,7 +5228,7 @@
         <v>3</v>
       </c>
       <c r="B690" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="691" spans="1:3" x14ac:dyDescent="0.25">
@@ -5309,7 +5318,7 @@
         <v>13</v>
       </c>
       <c r="C700" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="701" spans="1:3" x14ac:dyDescent="0.25">
@@ -5350,7 +5359,7 @@
         <v>4</v>
       </c>
       <c r="C705" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="706" spans="1:3" x14ac:dyDescent="0.25">
@@ -5391,7 +5400,7 @@
         <v>9</v>
       </c>
       <c r="C709" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="710" spans="1:3" x14ac:dyDescent="0.25">
@@ -5497,7 +5506,7 @@
     </row>
     <row r="723" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="724" spans="1:3" x14ac:dyDescent="0.25">
@@ -5511,11 +5520,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="725" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A725" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="726" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
         <v>5</v>
@@ -5554,7 +5558,7 @@
         <v>7</v>
       </c>
       <c r="C730" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="731" spans="1:3" x14ac:dyDescent="0.25">
@@ -5595,7 +5599,7 @@
         <v>6</v>
       </c>
       <c r="C734" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="735" spans="1:3" x14ac:dyDescent="0.25">
@@ -5628,11 +5632,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="739" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A739" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="740" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
         <v>3</v>
@@ -5646,7 +5645,7 @@
         <v>17</v>
       </c>
       <c r="C741" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="742" spans="1:3" x14ac:dyDescent="0.25">
@@ -5690,9 +5689,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="747" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A747" t="s">
-        <v>10</v>
+    <row r="747" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A747" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="748" spans="1:3" x14ac:dyDescent="0.25">
@@ -5703,7 +5702,7 @@
         <v>6</v>
       </c>
       <c r="C748" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="749" spans="1:3" x14ac:dyDescent="0.25">
@@ -5830,15 +5829,12 @@
         <v>7</v>
       </c>
       <c r="C768" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="769" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A769" t="s">
         <v>6</v>
-      </c>
-      <c r="B769" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="770" spans="1:3" x14ac:dyDescent="0.25">
@@ -5910,7 +5906,7 @@
         <v>5</v>
       </c>
       <c r="B779" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="780" spans="1:3" x14ac:dyDescent="0.25">
@@ -5982,7 +5978,7 @@
         <v>8</v>
       </c>
       <c r="C792" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="793" spans="1:3" x14ac:dyDescent="0.25">
@@ -5998,12 +5994,12 @@
     </row>
     <row r="794" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A794" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="795" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A795" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="799" spans="1:3" x14ac:dyDescent="0.25">
@@ -6173,7 +6169,7 @@
         <v>13</v>
       </c>
       <c r="C850" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="858" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>